<commit_message>
updated test cases excel file
</commit_message>
<xml_diff>
--- a/Documents/CLC-Project-test_Cases.xlsx
+++ b/Documents/CLC-Project-test_Cases.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="145">
   <si>
     <t>Project Name:</t>
   </si>
@@ -346,6 +346,108 @@
   </si>
   <si>
     <t xml:space="preserve">Verify the "Register" page is shown </t>
+  </si>
+  <si>
+    <t>Verifying the 'addBook' page with valid book inputs</t>
+  </si>
+  <si>
+    <t>"You must login before you can view the eBooks list!"</t>
+  </si>
+  <si>
+    <t>Navigate to the login page</t>
+  </si>
+  <si>
+    <t>Successfully navigated to the login page</t>
+  </si>
+  <si>
+    <t>Login using the correct credentials</t>
+  </si>
+  <si>
+    <t>username="username", password="password"</t>
+  </si>
+  <si>
+    <t>Login was successful</t>
+  </si>
+  <si>
+    <t>Ensure login success</t>
+  </si>
+  <si>
+    <t>Login Success page is shown</t>
+  </si>
+  <si>
+    <t>Navigate to addBook page</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/CLCProject/add</t>
+  </si>
+  <si>
+    <t>addBook.jsp</t>
+  </si>
+  <si>
+    <t>User was successfully navigated to the addBook page</t>
+  </si>
+  <si>
+    <t>Add a book to the database</t>
+  </si>
+  <si>
+    <t>Title="title", Author="author", isbn='978-0-446-31078-9', Publisher="publisher", Image='path-to-image'</t>
+  </si>
+  <si>
+    <t>addBookSuccess.jsp</t>
+  </si>
+  <si>
+    <t>Input parameters were successful</t>
+  </si>
+  <si>
+    <t>Verify success message is shown</t>
+  </si>
+  <si>
+    <t>Book was successfully added to the catalog</t>
+  </si>
+  <si>
+    <t>Verifying the 'addBook' page cannot be accessed without login</t>
+  </si>
+  <si>
+    <t>Navigate to the addBook page</t>
+  </si>
+  <si>
+    <t>Error Message was successfully displayed</t>
+  </si>
+  <si>
+    <t>Ensure user is redirected to the index page</t>
+  </si>
+  <si>
+    <t>User was successfully blocked from accessing addBook page, and was redirected to the index page</t>
+  </si>
+  <si>
+    <t>Verifying the 'bookList' page cannot be accessed without login</t>
+  </si>
+  <si>
+    <t>Navigate to the bookList page</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/CLCProject/bookList</t>
+  </si>
+  <si>
+    <t>User was successfully blocked from accessing bookList page, and was redirected to the index page</t>
+  </si>
+  <si>
+    <t>Verifying user cannot remove books from database without admin credentials</t>
+  </si>
+  <si>
+    <t>Navigate to the removeBook page</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/CLCProject/removeBook</t>
+  </si>
+  <si>
+    <t>You must have access to remove books from the database!</t>
+  </si>
+  <si>
+    <t>"You must have access to remove books from the database!"</t>
+  </si>
+  <si>
+    <t>User was successfully blocked from accessing removeBook page, and was redirected to the index page</t>
   </si>
 </sst>
 </file>
@@ -475,6 +577,11 @@
       <name val="Verdana"/>
     </font>
     <font>
+      <u/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <b/>
       <sz val="12.0"/>
       <name val="Times New Roman"/>
@@ -501,11 +608,6 @@
     <font>
       <b/>
       <name val="Verdana"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -700,7 +802,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="106">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -879,68 +981,79 @@
     </xf>
     <xf borderId="12" fillId="0" fontId="20" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="12" fillId="0" fontId="22" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="2" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="7" fillId="2" fontId="25" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="12" fillId="2" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="12" fillId="2" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="12" fillId="2" fontId="26" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="12" fillId="2" fontId="25" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="2" fontId="25" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="2" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="25" numFmtId="14" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="12" fillId="2" fontId="19" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="24" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="13" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="25" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="12" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="2" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="26" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="12" fillId="2" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="12" fillId="2" fontId="27" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="12" fillId="2" fontId="26" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="2" fontId="26" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="2" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="26" numFmtId="14" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="3" fillId="0" fontId="25" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="13" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="26" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="25" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="0" fontId="25" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="3" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="26" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="0" fontId="26" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="15" fillId="3" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="16" fillId="3" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="16" fillId="3" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="16" fillId="3" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="30" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="22" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1167,12 +1280,12 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="20.29"/>
-    <col customWidth="1" min="2" max="2" width="62.43"/>
-    <col customWidth="1" min="3" max="3" width="59.29"/>
-    <col customWidth="1" min="4" max="4" width="39.0"/>
-    <col customWidth="1" min="5" max="5" width="62.43"/>
+    <col customWidth="1" min="2" max="2" width="85.71"/>
+    <col customWidth="1" min="3" max="3" width="101.29"/>
+    <col customWidth="1" min="4" max="4" width="58.0"/>
+    <col customWidth="1" min="5" max="5" width="64.43"/>
     <col customWidth="1" min="6" max="6" width="18.29"/>
-    <col customWidth="1" min="7" max="7" width="68.0"/>
+    <col customWidth="1" min="7" max="7" width="102.57"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -2871,80 +2984,80 @@
       <c r="B108" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C108" s="74" t="s">
+      <c r="C108" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D108" s="74" t="s">
+      <c r="D108" s="40" t="s">
         <v>2</v>
       </c>
       <c r="E108" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="F108" s="75"/>
-      <c r="G108" s="76"/>
+      <c r="F108" s="42"/>
+      <c r="G108" s="43"/>
     </row>
     <row r="109" ht="12.75" customHeight="1">
       <c r="A109" s="7"/>
       <c r="B109" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C109" s="77" t="s">
+      <c r="C109" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="D109" s="78" t="s">
+      <c r="D109" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E109" s="79">
+      <c r="E109" s="46">
         <v>44351.0</v>
       </c>
-      <c r="F109" s="80"/>
-      <c r="G109" s="76"/>
+      <c r="F109" s="47"/>
+      <c r="G109" s="43"/>
     </row>
     <row r="110" ht="12.75" customHeight="1">
-      <c r="A110" s="81"/>
+      <c r="A110" s="48"/>
       <c r="B110" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C110" s="82">
+      <c r="C110" s="50">
         <v>1.0</v>
       </c>
-      <c r="D110" s="78" t="s">
+      <c r="D110" s="45" t="s">
         <v>8</v>
       </c>
       <c r="E110" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="F110" s="80"/>
-      <c r="G110" s="76"/>
+      <c r="F110" s="47"/>
+      <c r="G110" s="43"/>
     </row>
     <row r="111" ht="12.75" customHeight="1">
-      <c r="A111" s="83"/>
+      <c r="A111" s="52"/>
       <c r="B111" s="49"/>
-      <c r="C111" s="78"/>
-      <c r="D111" s="78" t="s">
+      <c r="C111" s="45"/>
+      <c r="D111" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="E111" s="84">
+      <c r="E111" s="53">
         <v>44353.0</v>
       </c>
-      <c r="F111" s="80"/>
-      <c r="G111" s="76"/>
+      <c r="F111" s="47"/>
+      <c r="G111" s="43"/>
     </row>
     <row r="112" ht="12.75" customHeight="1">
-      <c r="A112" s="85" t="s">
+      <c r="A112" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B112" s="86" t="s">
+      <c r="B112" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="C112" s="87"/>
-      <c r="D112" s="87"/>
-      <c r="E112" s="87"/>
-      <c r="F112" s="87"/>
-      <c r="G112" s="87"/>
+      <c r="C112" s="56"/>
+      <c r="D112" s="56"/>
+      <c r="E112" s="56"/>
+      <c r="F112" s="56"/>
+      <c r="G112" s="56"/>
     </row>
     <row r="113" ht="12.75" customHeight="1">
-      <c r="A113" s="88" t="s">
+      <c r="A113" s="57" t="s">
         <v>13</v>
       </c>
       <c r="B113" s="58" t="s">
@@ -2957,7 +3070,7 @@
       <c r="G113" s="60"/>
     </row>
     <row r="114" ht="12.75" customHeight="1">
-      <c r="A114" s="89" t="s">
+      <c r="A114" s="61" t="s">
         <v>15</v>
       </c>
       <c r="B114" s="58" t="s">
@@ -2970,52 +3083,52 @@
       <c r="G114" s="60"/>
     </row>
     <row r="115" ht="12.75" customHeight="1">
-      <c r="A115" s="89" t="s">
+      <c r="A115" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="B115" s="90" t="s">
+      <c r="B115" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="C115" s="76"/>
-      <c r="D115" s="76"/>
-      <c r="E115" s="76"/>
-      <c r="F115" s="76"/>
-      <c r="G115" s="76"/>
+      <c r="C115" s="43"/>
+      <c r="D115" s="43"/>
+      <c r="E115" s="43"/>
+      <c r="F115" s="43"/>
+      <c r="G115" s="43"/>
     </row>
     <row r="116" ht="12.75" customHeight="1">
-      <c r="A116" s="91"/>
-      <c r="B116" s="92"/>
-      <c r="C116" s="92"/>
-      <c r="D116" s="92"/>
-      <c r="E116" s="92"/>
-      <c r="F116" s="92"/>
-      <c r="G116" s="92"/>
+      <c r="A116" s="63"/>
+      <c r="B116" s="64"/>
+      <c r="C116" s="64"/>
+      <c r="D116" s="64"/>
+      <c r="E116" s="64"/>
+      <c r="F116" s="64"/>
+      <c r="G116" s="64"/>
     </row>
     <row r="117" ht="12.75" customHeight="1">
-      <c r="A117" s="93" t="s">
+      <c r="A117" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="B117" s="94" t="s">
+      <c r="B117" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C117" s="94" t="s">
+      <c r="C117" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="D117" s="94" t="s">
+      <c r="D117" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="E117" s="94" t="s">
+      <c r="E117" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="F117" s="94" t="s">
+      <c r="F117" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="G117" s="94" t="s">
+      <c r="G117" s="66" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="118" ht="12.75" customHeight="1">
-      <c r="A118" s="95">
+      <c r="A118" s="67">
         <v>1.0</v>
       </c>
       <c r="B118" s="68" t="s">
@@ -3024,62 +3137,62 @@
       <c r="C118" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D118" s="96" t="s">
+      <c r="D118" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="E118" s="96" t="s">
+      <c r="E118" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="F118" s="96" t="s">
+      <c r="F118" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G118" s="96" t="s">
+      <c r="G118" s="70" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="119" ht="12.75" customHeight="1">
-      <c r="A119" s="95">
+      <c r="A119" s="67">
         <v>2.0</v>
       </c>
-      <c r="B119" s="97" t="s">
+      <c r="B119" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C119" s="98" t="s">
+      <c r="C119" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="D119" s="97" t="s">
+      <c r="D119" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="E119" s="97" t="s">
+      <c r="E119" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="F119" s="96" t="s">
+      <c r="F119" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G119" s="97" t="s">
+      <c r="G119" s="70" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="120" ht="12.75" customHeight="1">
-      <c r="A120" s="95">
+      <c r="A120" s="67">
         <v>3.0</v>
       </c>
-      <c r="B120" s="97" t="s">
+      <c r="B120" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="C120" s="99" t="s">
+      <c r="C120" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="D120" s="97" t="s">
+      <c r="D120" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="E120" s="97" t="s">
+      <c r="E120" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="F120" s="96" t="s">
+      <c r="F120" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G120" s="97" t="s">
+      <c r="G120" s="70" t="s">
         <v>87</v>
       </c>
     </row>
@@ -3097,80 +3210,80 @@
       <c r="B122" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C122" s="74" t="s">
+      <c r="C122" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D122" s="74" t="s">
+      <c r="D122" s="40" t="s">
         <v>2</v>
       </c>
       <c r="E122" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="F122" s="75"/>
-      <c r="G122" s="76"/>
+      <c r="F122" s="42"/>
+      <c r="G122" s="43"/>
     </row>
     <row r="123" ht="12.75" customHeight="1">
       <c r="A123" s="7"/>
       <c r="B123" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C123" s="77" t="s">
+      <c r="C123" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="D123" s="78" t="s">
+      <c r="D123" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E123" s="79">
+      <c r="E123" s="46">
         <v>44351.0</v>
       </c>
-      <c r="F123" s="80"/>
-      <c r="G123" s="76"/>
+      <c r="F123" s="47"/>
+      <c r="G123" s="43"/>
     </row>
     <row r="124" ht="12.75" customHeight="1">
-      <c r="A124" s="81"/>
+      <c r="A124" s="48"/>
       <c r="B124" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C124" s="82">
+      <c r="C124" s="50">
         <v>1.0</v>
       </c>
-      <c r="D124" s="78" t="s">
+      <c r="D124" s="45" t="s">
         <v>8</v>
       </c>
       <c r="E124" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="F124" s="80"/>
-      <c r="G124" s="76"/>
+      <c r="F124" s="47"/>
+      <c r="G124" s="43"/>
     </row>
     <row r="125" ht="12.75" customHeight="1">
-      <c r="A125" s="83"/>
+      <c r="A125" s="52"/>
       <c r="B125" s="49"/>
-      <c r="C125" s="78"/>
-      <c r="D125" s="78" t="s">
+      <c r="C125" s="45"/>
+      <c r="D125" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="E125" s="84">
+      <c r="E125" s="53">
         <v>44353.0</v>
       </c>
-      <c r="F125" s="80"/>
-      <c r="G125" s="76"/>
+      <c r="F125" s="47"/>
+      <c r="G125" s="43"/>
     </row>
     <row r="126" ht="12.75" customHeight="1">
-      <c r="A126" s="85" t="s">
+      <c r="A126" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B126" s="86" t="s">
+      <c r="B126" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="C126" s="87"/>
-      <c r="D126" s="87"/>
-      <c r="E126" s="87"/>
-      <c r="F126" s="87"/>
-      <c r="G126" s="87"/>
+      <c r="C126" s="56"/>
+      <c r="D126" s="56"/>
+      <c r="E126" s="56"/>
+      <c r="F126" s="56"/>
+      <c r="G126" s="56"/>
     </row>
     <row r="127" ht="12.75" customHeight="1">
-      <c r="A127" s="88" t="s">
+      <c r="A127" s="57" t="s">
         <v>13</v>
       </c>
       <c r="B127" s="58" t="s">
@@ -3183,7 +3296,7 @@
       <c r="G127" s="60"/>
     </row>
     <row r="128" ht="12.75" customHeight="1">
-      <c r="A128" s="89" t="s">
+      <c r="A128" s="61" t="s">
         <v>15</v>
       </c>
       <c r="B128" s="58" t="s">
@@ -3196,52 +3309,52 @@
       <c r="G128" s="60"/>
     </row>
     <row r="129" ht="12.75" customHeight="1">
-      <c r="A129" s="89" t="s">
+      <c r="A129" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="B129" s="90" t="s">
+      <c r="B129" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="C129" s="76"/>
-      <c r="D129" s="76"/>
-      <c r="E129" s="76"/>
-      <c r="F129" s="76"/>
-      <c r="G129" s="76"/>
+      <c r="C129" s="43"/>
+      <c r="D129" s="43"/>
+      <c r="E129" s="43"/>
+      <c r="F129" s="43"/>
+      <c r="G129" s="43"/>
     </row>
     <row r="130" ht="12.75" customHeight="1">
-      <c r="A130" s="91"/>
-      <c r="B130" s="92"/>
-      <c r="C130" s="92"/>
-      <c r="D130" s="92"/>
-      <c r="E130" s="92"/>
-      <c r="F130" s="92"/>
-      <c r="G130" s="92"/>
+      <c r="A130" s="63"/>
+      <c r="B130" s="64"/>
+      <c r="C130" s="64"/>
+      <c r="D130" s="64"/>
+      <c r="E130" s="64"/>
+      <c r="F130" s="64"/>
+      <c r="G130" s="64"/>
     </row>
     <row r="131" ht="12.75" customHeight="1">
-      <c r="A131" s="93" t="s">
+      <c r="A131" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="B131" s="94" t="s">
+      <c r="B131" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C131" s="94" t="s">
+      <c r="C131" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="D131" s="94" t="s">
+      <c r="D131" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="E131" s="94" t="s">
+      <c r="E131" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="F131" s="94" t="s">
+      <c r="F131" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="G131" s="94" t="s">
+      <c r="G131" s="66" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="132" ht="12.75" customHeight="1">
-      <c r="A132" s="95">
+      <c r="A132" s="67">
         <v>1.0</v>
       </c>
       <c r="B132" s="68" t="s">
@@ -3250,85 +3363,85 @@
       <c r="C132" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D132" s="96" t="s">
+      <c r="D132" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="E132" s="96" t="s">
+      <c r="E132" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="F132" s="96" t="s">
+      <c r="F132" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G132" s="96" t="s">
+      <c r="G132" s="70" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="133" ht="12.75" customHeight="1">
-      <c r="A133" s="95">
+      <c r="A133" s="67">
         <v>2.0</v>
       </c>
-      <c r="B133" s="97" t="s">
+      <c r="B133" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C133" s="98" t="s">
+      <c r="C133" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="D133" s="97" t="s">
+      <c r="D133" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="E133" s="97" t="s">
+      <c r="E133" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="F133" s="96" t="s">
+      <c r="F133" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G133" s="97" t="s">
+      <c r="G133" s="70" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="134" ht="12.75" customHeight="1">
-      <c r="A134" s="95">
+      <c r="A134" s="67">
         <v>3.0</v>
       </c>
-      <c r="B134" s="97" t="s">
+      <c r="B134" s="70" t="s">
         <v>89</v>
       </c>
-      <c r="C134" s="99" t="s">
+      <c r="C134" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="D134" s="97" t="s">
+      <c r="D134" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="E134" s="97" t="s">
+      <c r="E134" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="F134" s="96" t="s">
+      <c r="F134" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G134" s="97" t="s">
+      <c r="G134" s="70" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="135" ht="12.75" customHeight="1">
-      <c r="A135" s="100">
+      <c r="A135" s="67">
         <v>4.0</v>
       </c>
-      <c r="B135" s="97" t="s">
+      <c r="B135" s="70" t="s">
         <v>93</v>
       </c>
-      <c r="C135" s="99" t="s">
+      <c r="C135" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="D135" s="97" t="s">
+      <c r="D135" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="E135" s="97" t="s">
+      <c r="E135" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="F135" s="97" t="s">
+      <c r="F135" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G135" s="97" t="s">
+      <c r="G135" s="70" t="s">
         <v>92</v>
       </c>
     </row>
@@ -3346,80 +3459,80 @@
       <c r="B137" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C137" s="74" t="s">
+      <c r="C137" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D137" s="74" t="s">
+      <c r="D137" s="40" t="s">
         <v>2</v>
       </c>
       <c r="E137" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="F137" s="75"/>
-      <c r="G137" s="76"/>
+      <c r="F137" s="42"/>
+      <c r="G137" s="43"/>
     </row>
     <row r="138" ht="12.75" customHeight="1">
       <c r="A138" s="7"/>
       <c r="B138" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C138" s="77" t="s">
+      <c r="C138" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="D138" s="78" t="s">
+      <c r="D138" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E138" s="79">
+      <c r="E138" s="46">
         <v>44351.0</v>
       </c>
-      <c r="F138" s="80"/>
-      <c r="G138" s="76"/>
+      <c r="F138" s="47"/>
+      <c r="G138" s="43"/>
     </row>
     <row r="139" ht="12.75" customHeight="1">
-      <c r="A139" s="81"/>
+      <c r="A139" s="48"/>
       <c r="B139" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C139" s="82">
+      <c r="C139" s="50">
         <v>1.0</v>
       </c>
-      <c r="D139" s="78" t="s">
+      <c r="D139" s="45" t="s">
         <v>8</v>
       </c>
       <c r="E139" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="F139" s="80"/>
-      <c r="G139" s="76"/>
+      <c r="F139" s="47"/>
+      <c r="G139" s="43"/>
     </row>
     <row r="140" ht="12.75" customHeight="1">
-      <c r="A140" s="83"/>
+      <c r="A140" s="52"/>
       <c r="B140" s="49"/>
-      <c r="C140" s="78"/>
-      <c r="D140" s="78" t="s">
+      <c r="C140" s="45"/>
+      <c r="D140" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="E140" s="84">
+      <c r="E140" s="53">
         <v>44353.0</v>
       </c>
-      <c r="F140" s="80"/>
-      <c r="G140" s="76"/>
+      <c r="F140" s="47"/>
+      <c r="G140" s="43"/>
     </row>
     <row r="141" ht="12.75" customHeight="1">
-      <c r="A141" s="85" t="s">
+      <c r="A141" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B141" s="86" t="s">
+      <c r="B141" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="C141" s="87"/>
-      <c r="D141" s="87"/>
-      <c r="E141" s="87"/>
-      <c r="F141" s="87"/>
-      <c r="G141" s="87"/>
+      <c r="C141" s="56"/>
+      <c r="D141" s="56"/>
+      <c r="E141" s="56"/>
+      <c r="F141" s="56"/>
+      <c r="G141" s="56"/>
     </row>
     <row r="142" ht="12.75" customHeight="1">
-      <c r="A142" s="88" t="s">
+      <c r="A142" s="57" t="s">
         <v>13</v>
       </c>
       <c r="B142" s="58" t="s">
@@ -3432,7 +3545,7 @@
       <c r="G142" s="60"/>
     </row>
     <row r="143" ht="12.75" customHeight="1">
-      <c r="A143" s="89" t="s">
+      <c r="A143" s="61" t="s">
         <v>15</v>
       </c>
       <c r="B143" s="58" t="s">
@@ -3445,52 +3558,52 @@
       <c r="G143" s="60"/>
     </row>
     <row r="144" ht="12.75" customHeight="1">
-      <c r="A144" s="89" t="s">
+      <c r="A144" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="B144" s="90" t="s">
+      <c r="B144" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="C144" s="76"/>
-      <c r="D144" s="76"/>
-      <c r="E144" s="76"/>
-      <c r="F144" s="76"/>
-      <c r="G144" s="76"/>
+      <c r="C144" s="43"/>
+      <c r="D144" s="43"/>
+      <c r="E144" s="43"/>
+      <c r="F144" s="43"/>
+      <c r="G144" s="43"/>
     </row>
     <row r="145" ht="12.75" customHeight="1">
-      <c r="A145" s="91"/>
-      <c r="B145" s="92"/>
-      <c r="C145" s="92"/>
-      <c r="D145" s="92"/>
-      <c r="E145" s="92"/>
-      <c r="F145" s="92"/>
-      <c r="G145" s="92"/>
+      <c r="A145" s="63"/>
+      <c r="B145" s="64"/>
+      <c r="C145" s="64"/>
+      <c r="D145" s="64"/>
+      <c r="E145" s="64"/>
+      <c r="F145" s="64"/>
+      <c r="G145" s="64"/>
     </row>
     <row r="146" ht="12.75" customHeight="1">
-      <c r="A146" s="93" t="s">
+      <c r="A146" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="B146" s="94" t="s">
+      <c r="B146" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C146" s="94" t="s">
+      <c r="C146" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="D146" s="94" t="s">
+      <c r="D146" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="E146" s="94" t="s">
+      <c r="E146" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="F146" s="94" t="s">
+      <c r="F146" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="G146" s="94" t="s">
+      <c r="G146" s="66" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="147" ht="12.75" customHeight="1">
-      <c r="A147" s="95">
+      <c r="A147" s="67">
         <v>1.0</v>
       </c>
       <c r="B147" s="68" t="s">
@@ -3499,85 +3612,85 @@
       <c r="C147" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D147" s="96" t="s">
+      <c r="D147" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="E147" s="96" t="s">
+      <c r="E147" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="F147" s="96" t="s">
+      <c r="F147" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G147" s="96" t="s">
+      <c r="G147" s="70" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="148" ht="12.75" customHeight="1">
-      <c r="A148" s="95">
+      <c r="A148" s="67">
         <v>2.0</v>
       </c>
-      <c r="B148" s="97" t="s">
+      <c r="B148" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C148" s="98" t="s">
+      <c r="C148" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="D148" s="97" t="s">
+      <c r="D148" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="E148" s="97" t="s">
+      <c r="E148" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="F148" s="96" t="s">
+      <c r="F148" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G148" s="97" t="s">
+      <c r="G148" s="70" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="149" ht="12.75" customHeight="1">
-      <c r="A149" s="95">
+      <c r="A149" s="67">
         <v>3.0</v>
       </c>
-      <c r="B149" s="97" t="s">
+      <c r="B149" s="70" t="s">
         <v>95</v>
       </c>
-      <c r="C149" s="99" t="s">
+      <c r="C149" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="D149" s="97" t="s">
+      <c r="D149" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="E149" s="97" t="s">
+      <c r="E149" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="F149" s="96" t="s">
+      <c r="F149" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G149" s="97" t="s">
+      <c r="G149" s="70" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="150" ht="12.75" customHeight="1">
-      <c r="A150" s="100">
+      <c r="A150" s="67">
         <v>4.0</v>
       </c>
-      <c r="B150" s="97" t="s">
+      <c r="B150" s="70" t="s">
         <v>99</v>
       </c>
-      <c r="C150" s="99" t="s">
+      <c r="C150" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="D150" s="97" t="s">
+      <c r="D150" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="E150" s="97" t="s">
+      <c r="E150" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="F150" s="97" t="s">
+      <c r="F150" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G150" s="97" t="s">
+      <c r="G150" s="70" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3595,80 +3708,80 @@
       <c r="B152" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C152" s="74" t="s">
+      <c r="C152" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D152" s="74" t="s">
+      <c r="D152" s="40" t="s">
         <v>2</v>
       </c>
       <c r="E152" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="F152" s="75"/>
-      <c r="G152" s="76"/>
+      <c r="F152" s="42"/>
+      <c r="G152" s="43"/>
     </row>
     <row r="153" ht="12.75" customHeight="1">
       <c r="A153" s="7"/>
       <c r="B153" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C153" s="77" t="s">
+      <c r="C153" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="D153" s="78" t="s">
+      <c r="D153" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E153" s="79">
+      <c r="E153" s="46">
         <v>44351.0</v>
       </c>
-      <c r="F153" s="80"/>
-      <c r="G153" s="76"/>
+      <c r="F153" s="47"/>
+      <c r="G153" s="43"/>
     </row>
     <row r="154" ht="12.75" customHeight="1">
-      <c r="A154" s="81"/>
+      <c r="A154" s="48"/>
       <c r="B154" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C154" s="82">
+      <c r="C154" s="50">
         <v>1.0</v>
       </c>
-      <c r="D154" s="78" t="s">
+      <c r="D154" s="45" t="s">
         <v>8</v>
       </c>
       <c r="E154" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="F154" s="80"/>
-      <c r="G154" s="76"/>
+      <c r="F154" s="47"/>
+      <c r="G154" s="43"/>
     </row>
     <row r="155" ht="12.75" customHeight="1">
-      <c r="A155" s="83"/>
+      <c r="A155" s="52"/>
       <c r="B155" s="49"/>
-      <c r="C155" s="78"/>
-      <c r="D155" s="78" t="s">
+      <c r="C155" s="45"/>
+      <c r="D155" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="E155" s="84">
+      <c r="E155" s="53">
         <v>44353.0</v>
       </c>
-      <c r="F155" s="80"/>
-      <c r="G155" s="76"/>
+      <c r="F155" s="47"/>
+      <c r="G155" s="43"/>
     </row>
     <row r="156" ht="12.75" customHeight="1">
-      <c r="A156" s="85" t="s">
+      <c r="A156" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B156" s="86" t="s">
+      <c r="B156" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="C156" s="87"/>
-      <c r="D156" s="87"/>
-      <c r="E156" s="87"/>
-      <c r="F156" s="87"/>
-      <c r="G156" s="87"/>
+      <c r="C156" s="56"/>
+      <c r="D156" s="56"/>
+      <c r="E156" s="56"/>
+      <c r="F156" s="56"/>
+      <c r="G156" s="56"/>
     </row>
     <row r="157" ht="12.75" customHeight="1">
-      <c r="A157" s="88" t="s">
+      <c r="A157" s="57" t="s">
         <v>13</v>
       </c>
       <c r="B157" s="58" t="s">
@@ -3681,7 +3794,7 @@
       <c r="G157" s="60"/>
     </row>
     <row r="158" ht="12.75" customHeight="1">
-      <c r="A158" s="89" t="s">
+      <c r="A158" s="61" t="s">
         <v>15</v>
       </c>
       <c r="B158" s="58" t="s">
@@ -3694,52 +3807,52 @@
       <c r="G158" s="60"/>
     </row>
     <row r="159" ht="12.75" customHeight="1">
-      <c r="A159" s="89" t="s">
+      <c r="A159" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="B159" s="90" t="s">
+      <c r="B159" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="C159" s="76"/>
-      <c r="D159" s="76"/>
-      <c r="E159" s="76"/>
-      <c r="F159" s="76"/>
-      <c r="G159" s="76"/>
+      <c r="C159" s="43"/>
+      <c r="D159" s="43"/>
+      <c r="E159" s="43"/>
+      <c r="F159" s="43"/>
+      <c r="G159" s="43"/>
     </row>
     <row r="160" ht="12.75" customHeight="1">
-      <c r="A160" s="91"/>
-      <c r="B160" s="92"/>
-      <c r="C160" s="92"/>
-      <c r="D160" s="92"/>
-      <c r="E160" s="92"/>
-      <c r="F160" s="92"/>
-      <c r="G160" s="92"/>
+      <c r="A160" s="63"/>
+      <c r="B160" s="64"/>
+      <c r="C160" s="64"/>
+      <c r="D160" s="64"/>
+      <c r="E160" s="64"/>
+      <c r="F160" s="64"/>
+      <c r="G160" s="64"/>
     </row>
     <row r="161" ht="12.75" customHeight="1">
-      <c r="A161" s="93" t="s">
+      <c r="A161" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="B161" s="94" t="s">
+      <c r="B161" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C161" s="94" t="s">
+      <c r="C161" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="D161" s="94" t="s">
+      <c r="D161" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="E161" s="94" t="s">
+      <c r="E161" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="F161" s="94" t="s">
+      <c r="F161" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="G161" s="94" t="s">
+      <c r="G161" s="66" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="162" ht="12.75" customHeight="1">
-      <c r="A162" s="95">
+      <c r="A162" s="67">
         <v>1.0</v>
       </c>
       <c r="B162" s="68" t="s">
@@ -3748,85 +3861,85 @@
       <c r="C162" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D162" s="96" t="s">
+      <c r="D162" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="E162" s="96" t="s">
+      <c r="E162" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="F162" s="96" t="s">
+      <c r="F162" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G162" s="96" t="s">
+      <c r="G162" s="70" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="163" ht="12.75" customHeight="1">
-      <c r="A163" s="95">
+      <c r="A163" s="67">
         <v>2.0</v>
       </c>
-      <c r="B163" s="97" t="s">
+      <c r="B163" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C163" s="98" t="s">
+      <c r="C163" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="D163" s="97" t="s">
+      <c r="D163" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="E163" s="97" t="s">
+      <c r="E163" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="F163" s="96" t="s">
+      <c r="F163" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G163" s="97" t="s">
+      <c r="G163" s="70" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="164" ht="12.75" customHeight="1">
-      <c r="A164" s="95">
+      <c r="A164" s="67">
         <v>3.0</v>
       </c>
-      <c r="B164" s="97" t="s">
+      <c r="B164" s="70" t="s">
         <v>101</v>
       </c>
-      <c r="C164" s="99" t="s">
+      <c r="C164" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="D164" s="97" t="s">
+      <c r="D164" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="E164" s="97" t="s">
+      <c r="E164" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="F164" s="96" t="s">
+      <c r="F164" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G164" s="97" t="s">
+      <c r="G164" s="70" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="165" ht="12.75" customHeight="1">
-      <c r="A165" s="100">
+      <c r="A165" s="67">
         <v>4.0</v>
       </c>
-      <c r="B165" s="97" t="s">
+      <c r="B165" s="70" t="s">
         <v>104</v>
       </c>
-      <c r="C165" s="99" t="s">
+      <c r="C165" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="D165" s="97" t="s">
+      <c r="D165" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="E165" s="97" t="s">
+      <c r="E165" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="F165" s="97" t="s">
+      <c r="F165" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G165" s="97" t="s">
+      <c r="G165" s="70" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3844,80 +3957,80 @@
       <c r="B167" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C167" s="74" t="s">
+      <c r="C167" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D167" s="74" t="s">
+      <c r="D167" s="40" t="s">
         <v>2</v>
       </c>
       <c r="E167" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="F167" s="75"/>
-      <c r="G167" s="76"/>
+      <c r="F167" s="42"/>
+      <c r="G167" s="43"/>
     </row>
     <row r="168" ht="12.75" customHeight="1">
       <c r="A168" s="7"/>
       <c r="B168" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C168" s="77" t="s">
+      <c r="C168" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="D168" s="78" t="s">
+      <c r="D168" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E168" s="79">
+      <c r="E168" s="46">
         <v>44351.0</v>
       </c>
-      <c r="F168" s="80"/>
-      <c r="G168" s="76"/>
+      <c r="F168" s="47"/>
+      <c r="G168" s="43"/>
     </row>
     <row r="169" ht="12.75" customHeight="1">
-      <c r="A169" s="81"/>
+      <c r="A169" s="48"/>
       <c r="B169" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C169" s="82">
+      <c r="C169" s="50">
         <v>1.0</v>
       </c>
-      <c r="D169" s="78" t="s">
+      <c r="D169" s="45" t="s">
         <v>8</v>
       </c>
       <c r="E169" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="F169" s="80"/>
-      <c r="G169" s="76"/>
+      <c r="F169" s="47"/>
+      <c r="G169" s="43"/>
     </row>
     <row r="170" ht="12.75" customHeight="1">
-      <c r="A170" s="83"/>
+      <c r="A170" s="52"/>
       <c r="B170" s="49"/>
-      <c r="C170" s="78"/>
-      <c r="D170" s="78" t="s">
+      <c r="C170" s="45"/>
+      <c r="D170" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="E170" s="84">
+      <c r="E170" s="53">
         <v>44353.0</v>
       </c>
-      <c r="F170" s="80"/>
-      <c r="G170" s="76"/>
+      <c r="F170" s="47"/>
+      <c r="G170" s="43"/>
     </row>
     <row r="171" ht="12.75" customHeight="1">
-      <c r="A171" s="85" t="s">
+      <c r="A171" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B171" s="86" t="s">
+      <c r="B171" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="C171" s="87"/>
-      <c r="D171" s="87"/>
-      <c r="E171" s="87"/>
-      <c r="F171" s="87"/>
-      <c r="G171" s="87"/>
+      <c r="C171" s="56"/>
+      <c r="D171" s="56"/>
+      <c r="E171" s="56"/>
+      <c r="F171" s="56"/>
+      <c r="G171" s="56"/>
     </row>
     <row r="172" ht="12.75" customHeight="1">
-      <c r="A172" s="88" t="s">
+      <c r="A172" s="57" t="s">
         <v>13</v>
       </c>
       <c r="B172" s="58" t="s">
@@ -3930,7 +4043,7 @@
       <c r="G172" s="60"/>
     </row>
     <row r="173" ht="12.75" customHeight="1">
-      <c r="A173" s="89" t="s">
+      <c r="A173" s="61" t="s">
         <v>15</v>
       </c>
       <c r="B173" s="58" t="s">
@@ -3943,52 +4056,52 @@
       <c r="G173" s="60"/>
     </row>
     <row r="174" ht="12.75" customHeight="1">
-      <c r="A174" s="89" t="s">
+      <c r="A174" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="B174" s="90" t="s">
+      <c r="B174" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="C174" s="76"/>
-      <c r="D174" s="76"/>
-      <c r="E174" s="76"/>
-      <c r="F174" s="76"/>
-      <c r="G174" s="76"/>
+      <c r="C174" s="43"/>
+      <c r="D174" s="43"/>
+      <c r="E174" s="43"/>
+      <c r="F174" s="43"/>
+      <c r="G174" s="43"/>
     </row>
     <row r="175" ht="12.75" customHeight="1">
-      <c r="A175" s="91"/>
-      <c r="B175" s="92"/>
-      <c r="C175" s="92"/>
-      <c r="D175" s="92"/>
-      <c r="E175" s="92"/>
-      <c r="F175" s="92"/>
-      <c r="G175" s="92"/>
+      <c r="A175" s="63"/>
+      <c r="B175" s="64"/>
+      <c r="C175" s="64"/>
+      <c r="D175" s="64"/>
+      <c r="E175" s="64"/>
+      <c r="F175" s="64"/>
+      <c r="G175" s="64"/>
     </row>
     <row r="176" ht="12.75" customHeight="1">
-      <c r="A176" s="93" t="s">
+      <c r="A176" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="B176" s="94" t="s">
+      <c r="B176" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C176" s="94" t="s">
+      <c r="C176" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="D176" s="94" t="s">
+      <c r="D176" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="E176" s="94" t="s">
+      <c r="E176" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="F176" s="94" t="s">
+      <c r="F176" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="G176" s="94" t="s">
+      <c r="G176" s="66" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="177" ht="12.75" customHeight="1">
-      <c r="A177" s="95">
+      <c r="A177" s="67">
         <v>1.0</v>
       </c>
       <c r="B177" s="68" t="s">
@@ -3997,85 +4110,85 @@
       <c r="C177" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D177" s="96" t="s">
+      <c r="D177" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="E177" s="96" t="s">
+      <c r="E177" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="F177" s="96" t="s">
+      <c r="F177" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G177" s="96" t="s">
+      <c r="G177" s="70" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="178" ht="12.75" customHeight="1">
-      <c r="A178" s="95">
+      <c r="A178" s="67">
         <v>2.0</v>
       </c>
-      <c r="B178" s="97" t="s">
+      <c r="B178" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C178" s="98" t="s">
+      <c r="C178" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="D178" s="97" t="s">
+      <c r="D178" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="E178" s="97" t="s">
+      <c r="E178" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="F178" s="96" t="s">
+      <c r="F178" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G178" s="97" t="s">
+      <c r="G178" s="70" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="179" ht="12.75" customHeight="1">
-      <c r="A179" s="95">
+      <c r="A179" s="67">
         <v>3.0</v>
       </c>
-      <c r="B179" s="97" t="s">
+      <c r="B179" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="C179" s="99" t="s">
+      <c r="C179" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="D179" s="97" t="s">
+      <c r="D179" s="70" t="s">
         <v>108</v>
       </c>
-      <c r="E179" s="97" t="s">
+      <c r="E179" s="70" t="s">
         <v>108</v>
       </c>
-      <c r="F179" s="96" t="s">
+      <c r="F179" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G179" s="97" t="s">
+      <c r="G179" s="70" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="180" ht="12.75" customHeight="1">
-      <c r="A180" s="100">
+      <c r="A180" s="67">
         <v>4.0</v>
       </c>
-      <c r="B180" s="97" t="s">
+      <c r="B180" s="70" t="s">
         <v>110</v>
       </c>
-      <c r="C180" s="99" t="s">
+      <c r="C180" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="D180" s="97" t="s">
+      <c r="D180" s="70" t="s">
         <v>108</v>
       </c>
-      <c r="E180" s="97" t="s">
+      <c r="E180" s="70" t="s">
         <v>108</v>
       </c>
-      <c r="F180" s="97" t="s">
+      <c r="F180" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G180" s="97" t="s">
+      <c r="G180" s="70" t="s">
         <v>109</v>
       </c>
     </row>
@@ -4098,157 +4211,313 @@
       <c r="G182" s="6"/>
     </row>
     <row r="183" ht="12.75" customHeight="1">
-      <c r="A183" s="6"/>
-      <c r="B183" s="35"/>
-      <c r="C183" s="6"/>
-      <c r="D183" s="6"/>
-      <c r="E183" s="6"/>
-      <c r="F183" s="6"/>
-      <c r="G183" s="6"/>
+      <c r="A183" s="38"/>
+      <c r="B183" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C183" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="D183" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="E183" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="F183" s="76"/>
+      <c r="G183" s="77"/>
     </row>
     <row r="184" ht="12.75" customHeight="1">
-      <c r="A184" s="6"/>
-      <c r="B184" s="35"/>
-      <c r="C184" s="6"/>
-      <c r="D184" s="6"/>
-      <c r="E184" s="6"/>
-      <c r="F184" s="6"/>
-      <c r="G184" s="6"/>
+      <c r="A184" s="7"/>
+      <c r="B184" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C184" s="78" t="s">
+        <v>80</v>
+      </c>
+      <c r="D184" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="E184" s="79">
+        <v>44351.0</v>
+      </c>
+      <c r="F184" s="80"/>
+      <c r="G184" s="77"/>
     </row>
     <row r="185" ht="12.75" customHeight="1">
-      <c r="A185" s="6"/>
-      <c r="B185" s="35"/>
-      <c r="C185" s="6"/>
-      <c r="D185" s="6"/>
-      <c r="E185" s="6"/>
-      <c r="F185" s="6"/>
-      <c r="G185" s="6"/>
+      <c r="A185" s="81"/>
+      <c r="B185" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C185" s="82">
+        <v>1.0</v>
+      </c>
+      <c r="D185" s="78" t="s">
+        <v>8</v>
+      </c>
+      <c r="E185" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F185" s="80"/>
+      <c r="G185" s="77"/>
     </row>
     <row r="186" ht="12.75" customHeight="1">
-      <c r="A186" s="6"/>
-      <c r="B186" s="35"/>
-      <c r="C186" s="6"/>
-      <c r="D186" s="6"/>
-      <c r="E186" s="6"/>
-      <c r="F186" s="6"/>
-      <c r="G186" s="6"/>
+      <c r="A186" s="83"/>
+      <c r="B186" s="49"/>
+      <c r="C186" s="78"/>
+      <c r="D186" s="78" t="s">
+        <v>10</v>
+      </c>
+      <c r="E186" s="53">
+        <v>44353.0</v>
+      </c>
+      <c r="F186" s="80"/>
+      <c r="G186" s="77"/>
     </row>
     <row r="187" ht="12.75" customHeight="1">
-      <c r="A187" s="6"/>
-      <c r="B187" s="35"/>
-      <c r="C187" s="6"/>
-      <c r="D187" s="6"/>
-      <c r="E187" s="6"/>
-      <c r="F187" s="6"/>
-      <c r="G187" s="6"/>
+      <c r="A187" s="84" t="s">
+        <v>11</v>
+      </c>
+      <c r="B187" s="85" t="s">
+        <v>111</v>
+      </c>
+      <c r="C187" s="86"/>
+      <c r="D187" s="86"/>
+      <c r="E187" s="86"/>
+      <c r="F187" s="86"/>
+      <c r="G187" s="86"/>
     </row>
     <row r="188" ht="12.75" customHeight="1">
-      <c r="A188" s="6"/>
-      <c r="B188" s="35"/>
-      <c r="C188" s="6"/>
-      <c r="D188" s="6"/>
-      <c r="E188" s="6"/>
-      <c r="F188" s="6"/>
-      <c r="G188" s="6"/>
+      <c r="A188" s="87" t="s">
+        <v>13</v>
+      </c>
+      <c r="B188" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="C188" s="59"/>
+      <c r="D188" s="59"/>
+      <c r="E188" s="59"/>
+      <c r="F188" s="59"/>
+      <c r="G188" s="60"/>
     </row>
     <row r="189" ht="12.75" customHeight="1">
-      <c r="A189" s="6"/>
-      <c r="B189" s="35"/>
-      <c r="C189" s="6"/>
-      <c r="D189" s="6"/>
-      <c r="E189" s="6"/>
-      <c r="F189" s="6"/>
-      <c r="G189" s="6"/>
+      <c r="A189" s="88" t="s">
+        <v>15</v>
+      </c>
+      <c r="B189" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="C189" s="59"/>
+      <c r="D189" s="59"/>
+      <c r="E189" s="59"/>
+      <c r="F189" s="59"/>
+      <c r="G189" s="60"/>
     </row>
     <row r="190" ht="12.75" customHeight="1">
-      <c r="A190" s="6"/>
-      <c r="B190" s="35"/>
-      <c r="C190" s="6"/>
-      <c r="D190" s="6"/>
-      <c r="E190" s="6"/>
-      <c r="F190" s="6"/>
-      <c r="G190" s="6"/>
+      <c r="A190" s="88" t="s">
+        <v>17</v>
+      </c>
+      <c r="B190" s="89" t="s">
+        <v>18</v>
+      </c>
+      <c r="C190" s="77"/>
+      <c r="D190" s="77"/>
+      <c r="E190" s="77"/>
+      <c r="F190" s="77"/>
+      <c r="G190" s="77"/>
     </row>
     <row r="191" ht="12.75" customHeight="1">
-      <c r="A191" s="6"/>
-      <c r="B191" s="35"/>
-      <c r="C191" s="6"/>
-      <c r="D191" s="6"/>
-      <c r="E191" s="6"/>
-      <c r="F191" s="6"/>
-      <c r="G191" s="6"/>
+      <c r="A191" s="90"/>
+      <c r="B191" s="91"/>
+      <c r="C191" s="91"/>
+      <c r="D191" s="91"/>
+      <c r="E191" s="91"/>
+      <c r="F191" s="91"/>
+      <c r="G191" s="91"/>
     </row>
     <row r="192" ht="12.75" customHeight="1">
-      <c r="A192" s="6"/>
-      <c r="B192" s="35"/>
-      <c r="C192" s="6"/>
-      <c r="D192" s="6"/>
-      <c r="E192" s="6"/>
-      <c r="F192" s="6"/>
-      <c r="G192" s="6"/>
+      <c r="A192" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="B192" s="93" t="s">
+        <v>20</v>
+      </c>
+      <c r="C192" s="93" t="s">
+        <v>21</v>
+      </c>
+      <c r="D192" s="94" t="s">
+        <v>112</v>
+      </c>
+      <c r="E192" s="93" t="s">
+        <v>23</v>
+      </c>
+      <c r="F192" s="93" t="s">
+        <v>24</v>
+      </c>
+      <c r="G192" s="93" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="193" ht="12.75" customHeight="1">
-      <c r="A193" s="6"/>
-      <c r="B193" s="35"/>
-      <c r="C193" s="6"/>
-      <c r="D193" s="6"/>
-      <c r="E193" s="6"/>
-      <c r="F193" s="6"/>
-      <c r="G193" s="6"/>
+      <c r="A193" s="95">
+        <v>1.0</v>
+      </c>
+      <c r="B193" s="68" t="s">
+        <v>26</v>
+      </c>
+      <c r="C193" s="69" t="s">
+        <v>27</v>
+      </c>
+      <c r="D193" s="96" t="s">
+        <v>28</v>
+      </c>
+      <c r="E193" s="96" t="s">
+        <v>28</v>
+      </c>
+      <c r="F193" s="96" t="s">
+        <v>29</v>
+      </c>
+      <c r="G193" s="96" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="194" ht="12.75" customHeight="1">
-      <c r="A194" s="6"/>
-      <c r="B194" s="35"/>
-      <c r="C194" s="6"/>
-      <c r="D194" s="6"/>
-      <c r="E194" s="6"/>
-      <c r="F194" s="6"/>
-      <c r="G194" s="6"/>
+      <c r="A194" s="95">
+        <v>2.0</v>
+      </c>
+      <c r="B194" s="97" t="s">
+        <v>113</v>
+      </c>
+      <c r="C194" s="98" t="s">
+        <v>32</v>
+      </c>
+      <c r="D194" s="97" t="s">
+        <v>64</v>
+      </c>
+      <c r="E194" s="97" t="s">
+        <v>64</v>
+      </c>
+      <c r="F194" s="96" t="s">
+        <v>29</v>
+      </c>
+      <c r="G194" s="97" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="195" ht="12.75" customHeight="1">
-      <c r="A195" s="6"/>
-      <c r="B195" s="35"/>
-      <c r="C195" s="6"/>
-      <c r="D195" s="6"/>
-      <c r="E195" s="6"/>
-      <c r="F195" s="6"/>
-      <c r="G195" s="6"/>
+      <c r="A195" s="95">
+        <v>3.0</v>
+      </c>
+      <c r="B195" s="97" t="s">
+        <v>115</v>
+      </c>
+      <c r="C195" s="99" t="s">
+        <v>116</v>
+      </c>
+      <c r="D195" s="97" t="s">
+        <v>64</v>
+      </c>
+      <c r="E195" s="97" t="s">
+        <v>64</v>
+      </c>
+      <c r="F195" s="96" t="s">
+        <v>29</v>
+      </c>
+      <c r="G195" s="97" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="196" ht="12.75" customHeight="1">
-      <c r="A196" s="6"/>
-      <c r="B196" s="35"/>
-      <c r="C196" s="6"/>
-      <c r="D196" s="6"/>
-      <c r="E196" s="6"/>
-      <c r="F196" s="6"/>
-      <c r="G196" s="6"/>
+      <c r="A196" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="B196" s="97" t="s">
+        <v>118</v>
+      </c>
+      <c r="C196" s="100" t="s">
+        <v>16</v>
+      </c>
+      <c r="D196" s="97" t="s">
+        <v>67</v>
+      </c>
+      <c r="E196" s="97" t="s">
+        <v>67</v>
+      </c>
+      <c r="F196" s="96" t="s">
+        <v>29</v>
+      </c>
+      <c r="G196" s="97" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="197" ht="12.75" customHeight="1">
-      <c r="A197" s="6"/>
-      <c r="B197" s="35"/>
-      <c r="C197" s="6"/>
-      <c r="D197" s="6"/>
-      <c r="E197" s="6"/>
-      <c r="F197" s="6"/>
-      <c r="G197" s="6"/>
+      <c r="A197" s="101">
+        <v>5.0</v>
+      </c>
+      <c r="B197" s="97" t="s">
+        <v>120</v>
+      </c>
+      <c r="C197" s="102" t="s">
+        <v>121</v>
+      </c>
+      <c r="D197" s="97" t="s">
+        <v>122</v>
+      </c>
+      <c r="E197" s="97" t="s">
+        <v>122</v>
+      </c>
+      <c r="F197" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="G197" s="97" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="198" ht="12.75" customHeight="1">
-      <c r="A198" s="6"/>
-      <c r="B198" s="35"/>
-      <c r="C198" s="6"/>
-      <c r="D198" s="6"/>
-      <c r="E198" s="6"/>
-      <c r="F198" s="6"/>
-      <c r="G198" s="6"/>
+      <c r="A198" s="101">
+        <v>6.0</v>
+      </c>
+      <c r="B198" s="97" t="s">
+        <v>124</v>
+      </c>
+      <c r="C198" s="99" t="s">
+        <v>125</v>
+      </c>
+      <c r="D198" s="97" t="s">
+        <v>126</v>
+      </c>
+      <c r="E198" s="97" t="s">
+        <v>126</v>
+      </c>
+      <c r="F198" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="G198" s="97" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="199" ht="12.75" customHeight="1">
-      <c r="A199" s="6"/>
-      <c r="B199" s="35"/>
-      <c r="C199" s="6"/>
-      <c r="D199" s="6"/>
-      <c r="E199" s="6"/>
-      <c r="F199" s="6"/>
-      <c r="G199" s="6"/>
+      <c r="A199" s="101">
+        <v>7.0</v>
+      </c>
+      <c r="B199" s="97" t="s">
+        <v>128</v>
+      </c>
+      <c r="C199" s="99" t="s">
+        <v>16</v>
+      </c>
+      <c r="D199" s="97" t="s">
+        <v>126</v>
+      </c>
+      <c r="E199" s="97" t="s">
+        <v>126</v>
+      </c>
+      <c r="F199" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="G199" s="97" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="200" ht="12.75" customHeight="1">
       <c r="A200" s="6"/>
@@ -4269,121 +4538,221 @@
       <c r="G201" s="6"/>
     </row>
     <row r="202" ht="12.75" customHeight="1">
-      <c r="A202" s="6"/>
-      <c r="B202" s="35"/>
-      <c r="C202" s="6"/>
-      <c r="D202" s="6"/>
-      <c r="E202" s="6"/>
-      <c r="F202" s="6"/>
-      <c r="G202" s="6"/>
+      <c r="A202" s="38"/>
+      <c r="B202" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C202" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="D202" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="E202" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="F202" s="76"/>
+      <c r="G202" s="77"/>
     </row>
     <row r="203" ht="12.75" customHeight="1">
-      <c r="A203" s="6"/>
-      <c r="B203" s="35"/>
-      <c r="C203" s="6"/>
-      <c r="D203" s="6"/>
-      <c r="E203" s="6"/>
-      <c r="F203" s="6"/>
-      <c r="G203" s="6"/>
+      <c r="A203" s="7"/>
+      <c r="B203" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C203" s="78" t="s">
+        <v>80</v>
+      </c>
+      <c r="D203" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="E203" s="79">
+        <v>44351.0</v>
+      </c>
+      <c r="F203" s="80"/>
+      <c r="G203" s="77"/>
     </row>
     <row r="204" ht="12.75" customHeight="1">
-      <c r="A204" s="6"/>
-      <c r="B204" s="35"/>
-      <c r="C204" s="6"/>
-      <c r="D204" s="6"/>
-      <c r="E204" s="6"/>
-      <c r="F204" s="6"/>
-      <c r="G204" s="6"/>
+      <c r="A204" s="81"/>
+      <c r="B204" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C204" s="82">
+        <v>1.0</v>
+      </c>
+      <c r="D204" s="78" t="s">
+        <v>8</v>
+      </c>
+      <c r="E204" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F204" s="80"/>
+      <c r="G204" s="77"/>
     </row>
     <row r="205" ht="12.75" customHeight="1">
-      <c r="A205" s="6"/>
-      <c r="B205" s="35"/>
-      <c r="C205" s="6"/>
-      <c r="D205" s="6"/>
-      <c r="E205" s="6"/>
-      <c r="F205" s="6"/>
-      <c r="G205" s="6"/>
+      <c r="A205" s="83"/>
+      <c r="B205" s="49"/>
+      <c r="C205" s="78"/>
+      <c r="D205" s="78" t="s">
+        <v>10</v>
+      </c>
+      <c r="E205" s="53">
+        <v>44353.0</v>
+      </c>
+      <c r="F205" s="80"/>
+      <c r="G205" s="77"/>
     </row>
     <row r="206" ht="12.75" customHeight="1">
-      <c r="A206" s="6"/>
-      <c r="B206" s="35"/>
-      <c r="C206" s="6"/>
-      <c r="D206" s="6"/>
-      <c r="E206" s="6"/>
-      <c r="F206" s="6"/>
-      <c r="G206" s="6"/>
+      <c r="A206" s="84" t="s">
+        <v>11</v>
+      </c>
+      <c r="B206" s="85" t="s">
+        <v>130</v>
+      </c>
+      <c r="C206" s="86"/>
+      <c r="D206" s="86"/>
+      <c r="E206" s="86"/>
+      <c r="F206" s="86"/>
+      <c r="G206" s="86"/>
     </row>
     <row r="207" ht="12.75" customHeight="1">
-      <c r="A207" s="6"/>
-      <c r="B207" s="35"/>
-      <c r="C207" s="6"/>
-      <c r="D207" s="6"/>
-      <c r="E207" s="6"/>
-      <c r="F207" s="6"/>
-      <c r="G207" s="6"/>
+      <c r="A207" s="87" t="s">
+        <v>13</v>
+      </c>
+      <c r="B207" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="C207" s="59"/>
+      <c r="D207" s="59"/>
+      <c r="E207" s="59"/>
+      <c r="F207" s="59"/>
+      <c r="G207" s="60"/>
     </row>
     <row r="208" ht="12.75" customHeight="1">
-      <c r="A208" s="6"/>
-      <c r="B208" s="35"/>
-      <c r="C208" s="6"/>
-      <c r="D208" s="6"/>
-      <c r="E208" s="6"/>
-      <c r="F208" s="6"/>
-      <c r="G208" s="6"/>
+      <c r="A208" s="88" t="s">
+        <v>15</v>
+      </c>
+      <c r="B208" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="C208" s="59"/>
+      <c r="D208" s="59"/>
+      <c r="E208" s="59"/>
+      <c r="F208" s="59"/>
+      <c r="G208" s="60"/>
     </row>
     <row r="209" ht="12.75" customHeight="1">
-      <c r="A209" s="6"/>
-      <c r="B209" s="35"/>
-      <c r="C209" s="6"/>
-      <c r="D209" s="6"/>
-      <c r="E209" s="6"/>
-      <c r="F209" s="6"/>
-      <c r="G209" s="6"/>
+      <c r="A209" s="88" t="s">
+        <v>17</v>
+      </c>
+      <c r="B209" s="89" t="s">
+        <v>18</v>
+      </c>
+      <c r="C209" s="77"/>
+      <c r="D209" s="77"/>
+      <c r="E209" s="77"/>
+      <c r="F209" s="77"/>
+      <c r="G209" s="77"/>
     </row>
     <row r="210" ht="12.75" customHeight="1">
-      <c r="A210" s="6"/>
-      <c r="B210" s="35"/>
-      <c r="C210" s="6"/>
-      <c r="D210" s="6"/>
-      <c r="E210" s="6"/>
-      <c r="F210" s="6"/>
-      <c r="G210" s="6"/>
+      <c r="A210" s="90"/>
+      <c r="B210" s="91"/>
+      <c r="C210" s="91"/>
+      <c r="D210" s="91"/>
+      <c r="E210" s="91"/>
+      <c r="F210" s="91"/>
+      <c r="G210" s="91"/>
     </row>
     <row r="211" ht="12.75" customHeight="1">
-      <c r="A211" s="6"/>
-      <c r="B211" s="35"/>
-      <c r="C211" s="6"/>
-      <c r="D211" s="6"/>
-      <c r="E211" s="6"/>
-      <c r="F211" s="6"/>
-      <c r="G211" s="6"/>
+      <c r="A211" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="B211" s="93" t="s">
+        <v>20</v>
+      </c>
+      <c r="C211" s="93" t="s">
+        <v>21</v>
+      </c>
+      <c r="D211" s="93" t="s">
+        <v>22</v>
+      </c>
+      <c r="E211" s="93" t="s">
+        <v>23</v>
+      </c>
+      <c r="F211" s="93" t="s">
+        <v>24</v>
+      </c>
+      <c r="G211" s="93" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="212" ht="12.75" customHeight="1">
-      <c r="A212" s="6"/>
-      <c r="B212" s="35"/>
-      <c r="C212" s="6"/>
-      <c r="D212" s="6"/>
-      <c r="E212" s="6"/>
-      <c r="F212" s="6"/>
-      <c r="G212" s="6"/>
+      <c r="A212" s="95">
+        <v>1.0</v>
+      </c>
+      <c r="B212" s="68" t="s">
+        <v>26</v>
+      </c>
+      <c r="C212" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="D212" s="96" t="s">
+        <v>28</v>
+      </c>
+      <c r="E212" s="96" t="s">
+        <v>28</v>
+      </c>
+      <c r="F212" s="96" t="s">
+        <v>29</v>
+      </c>
+      <c r="G212" s="96" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="213" ht="12.75" customHeight="1">
-      <c r="A213" s="6"/>
-      <c r="B213" s="35"/>
-      <c r="C213" s="6"/>
-      <c r="D213" s="6"/>
-      <c r="E213" s="6"/>
-      <c r="F213" s="6"/>
-      <c r="G213" s="6"/>
+      <c r="A213" s="95">
+        <v>2.0</v>
+      </c>
+      <c r="B213" s="97" t="s">
+        <v>131</v>
+      </c>
+      <c r="C213" s="98" t="s">
+        <v>121</v>
+      </c>
+      <c r="D213" s="97" t="s">
+        <v>112</v>
+      </c>
+      <c r="E213" s="97" t="s">
+        <v>112</v>
+      </c>
+      <c r="F213" s="96" t="s">
+        <v>29</v>
+      </c>
+      <c r="G213" s="97" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="214" ht="12.75" customHeight="1">
-      <c r="A214" s="6"/>
-      <c r="B214" s="35"/>
-      <c r="C214" s="6"/>
-      <c r="D214" s="6"/>
-      <c r="E214" s="6"/>
-      <c r="F214" s="6"/>
-      <c r="G214" s="6"/>
+      <c r="A214" s="95">
+        <v>3.0</v>
+      </c>
+      <c r="B214" s="97" t="s">
+        <v>133</v>
+      </c>
+      <c r="C214" s="99" t="s">
+        <v>16</v>
+      </c>
+      <c r="D214" s="97" t="s">
+        <v>28</v>
+      </c>
+      <c r="E214" s="97" t="s">
+        <v>28</v>
+      </c>
+      <c r="F214" s="96" t="s">
+        <v>29</v>
+      </c>
+      <c r="G214" s="97" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="215" ht="12.75" customHeight="1">
       <c r="A215" s="6"/>
@@ -4404,41 +4773,441 @@
       <c r="G216" s="6"/>
     </row>
     <row r="217" ht="12.75" customHeight="1">
-      <c r="A217" s="6"/>
-      <c r="B217" s="35"/>
-      <c r="C217" s="6"/>
-      <c r="D217" s="6"/>
-      <c r="E217" s="6"/>
-      <c r="F217" s="6"/>
-      <c r="G217" s="6"/>
-    </row>
-    <row r="218" ht="12.75" customHeight="1"/>
-    <row r="219" ht="12.75" customHeight="1"/>
-    <row r="220" ht="12.75" customHeight="1"/>
-    <row r="221" ht="12.75" customHeight="1"/>
-    <row r="222" ht="12.75" customHeight="1"/>
-    <row r="223" ht="12.75" customHeight="1"/>
-    <row r="224" ht="12.75" customHeight="1"/>
-    <row r="225" ht="12.75" customHeight="1"/>
-    <row r="226" ht="12.75" customHeight="1"/>
-    <row r="227" ht="12.75" customHeight="1"/>
-    <row r="228" ht="12.75" customHeight="1"/>
-    <row r="229" ht="12.75" customHeight="1"/>
+      <c r="A217" s="38"/>
+      <c r="B217" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C217" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D217" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="E217" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="F217" s="42"/>
+      <c r="G217" s="43"/>
+    </row>
+    <row r="218" ht="12.75" customHeight="1">
+      <c r="A218" s="7"/>
+      <c r="B218" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C218" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="D218" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E218" s="46">
+        <v>44351.0</v>
+      </c>
+      <c r="F218" s="47"/>
+      <c r="G218" s="43"/>
+    </row>
+    <row r="219" ht="12.75" customHeight="1">
+      <c r="A219" s="48"/>
+      <c r="B219" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C219" s="50">
+        <v>1.0</v>
+      </c>
+      <c r="D219" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E219" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F219" s="47"/>
+      <c r="G219" s="43"/>
+    </row>
+    <row r="220" ht="12.75" customHeight="1">
+      <c r="A220" s="52"/>
+      <c r="B220" s="49"/>
+      <c r="C220" s="45"/>
+      <c r="D220" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="E220" s="53">
+        <v>44353.0</v>
+      </c>
+      <c r="F220" s="47"/>
+      <c r="G220" s="43"/>
+    </row>
+    <row r="221" ht="12.75" customHeight="1">
+      <c r="A221" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="B221" s="85" t="s">
+        <v>135</v>
+      </c>
+      <c r="C221" s="56"/>
+      <c r="D221" s="56"/>
+      <c r="E221" s="56"/>
+      <c r="F221" s="56"/>
+      <c r="G221" s="56"/>
+    </row>
+    <row r="222" ht="12.75" customHeight="1">
+      <c r="A222" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="B222" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="C222" s="59"/>
+      <c r="D222" s="59"/>
+      <c r="E222" s="59"/>
+      <c r="F222" s="59"/>
+      <c r="G222" s="60"/>
+    </row>
+    <row r="223" ht="12.75" customHeight="1">
+      <c r="A223" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="B223" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="C223" s="59"/>
+      <c r="D223" s="59"/>
+      <c r="E223" s="59"/>
+      <c r="F223" s="59"/>
+      <c r="G223" s="60"/>
+    </row>
+    <row r="224" ht="12.75" customHeight="1">
+      <c r="A224" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="B224" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="C224" s="43"/>
+      <c r="D224" s="43"/>
+      <c r="E224" s="43"/>
+      <c r="F224" s="43"/>
+      <c r="G224" s="43"/>
+    </row>
+    <row r="225" ht="12.75" customHeight="1">
+      <c r="A225" s="63"/>
+      <c r="B225" s="64"/>
+      <c r="C225" s="64"/>
+      <c r="D225" s="64"/>
+      <c r="E225" s="64"/>
+      <c r="F225" s="64"/>
+      <c r="G225" s="64"/>
+    </row>
+    <row r="226" ht="12.75" customHeight="1">
+      <c r="A226" s="65" t="s">
+        <v>19</v>
+      </c>
+      <c r="B226" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="C226" s="66" t="s">
+        <v>21</v>
+      </c>
+      <c r="D226" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="E226" s="66" t="s">
+        <v>23</v>
+      </c>
+      <c r="F226" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="G226" s="66" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="227" ht="12.75" customHeight="1">
+      <c r="A227" s="67">
+        <v>1.0</v>
+      </c>
+      <c r="B227" s="68" t="s">
+        <v>26</v>
+      </c>
+      <c r="C227" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="D227" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="E227" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="F227" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="G227" s="70" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="228" ht="12.75" customHeight="1">
+      <c r="A228" s="67">
+        <v>2.0</v>
+      </c>
+      <c r="B228" s="97" t="s">
+        <v>136</v>
+      </c>
+      <c r="C228" s="98" t="s">
+        <v>137</v>
+      </c>
+      <c r="D228" s="104" t="s">
+        <v>112</v>
+      </c>
+      <c r="E228" s="104" t="s">
+        <v>112</v>
+      </c>
+      <c r="F228" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="G228" s="104" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="229" ht="12.75" customHeight="1">
+      <c r="A229" s="67">
+        <v>3.0</v>
+      </c>
+      <c r="B229" s="104" t="s">
+        <v>133</v>
+      </c>
+      <c r="C229" s="105" t="s">
+        <v>16</v>
+      </c>
+      <c r="D229" s="104" t="s">
+        <v>28</v>
+      </c>
+      <c r="E229" s="104" t="s">
+        <v>28</v>
+      </c>
+      <c r="F229" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="G229" s="97" t="s">
+        <v>138</v>
+      </c>
+    </row>
     <row r="230" ht="12.75" customHeight="1"/>
     <row r="231" ht="12.75" customHeight="1"/>
-    <row r="232" ht="12.75" customHeight="1"/>
-    <row r="233" ht="12.75" customHeight="1"/>
-    <row r="234" ht="12.75" customHeight="1"/>
-    <row r="235" ht="12.75" customHeight="1"/>
-    <row r="236" ht="12.75" customHeight="1"/>
-    <row r="237" ht="12.75" customHeight="1"/>
-    <row r="238" ht="12.75" customHeight="1"/>
-    <row r="239" ht="12.75" customHeight="1"/>
-    <row r="240" ht="12.75" customHeight="1"/>
-    <row r="241" ht="12.75" customHeight="1"/>
-    <row r="242" ht="12.75" customHeight="1"/>
-    <row r="243" ht="12.75" customHeight="1"/>
-    <row r="244" ht="12.75" customHeight="1"/>
+    <row r="232" ht="12.75" customHeight="1">
+      <c r="A232" s="38"/>
+      <c r="B232" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C232" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D232" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="E232" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="F232" s="42"/>
+      <c r="G232" s="43"/>
+    </row>
+    <row r="233" ht="12.75" customHeight="1">
+      <c r="A233" s="7"/>
+      <c r="B233" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C233" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="D233" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E233" s="46">
+        <v>44351.0</v>
+      </c>
+      <c r="F233" s="47"/>
+      <c r="G233" s="43"/>
+    </row>
+    <row r="234" ht="12.75" customHeight="1">
+      <c r="A234" s="48"/>
+      <c r="B234" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C234" s="50">
+        <v>1.0</v>
+      </c>
+      <c r="D234" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E234" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F234" s="47"/>
+      <c r="G234" s="43"/>
+    </row>
+    <row r="235" ht="12.75" customHeight="1">
+      <c r="A235" s="52"/>
+      <c r="B235" s="49"/>
+      <c r="C235" s="45"/>
+      <c r="D235" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="E235" s="53">
+        <v>44353.0</v>
+      </c>
+      <c r="F235" s="47"/>
+      <c r="G235" s="43"/>
+    </row>
+    <row r="236" ht="12.75" customHeight="1">
+      <c r="A236" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="B236" s="85" t="s">
+        <v>139</v>
+      </c>
+      <c r="C236" s="56"/>
+      <c r="D236" s="56"/>
+      <c r="E236" s="56"/>
+      <c r="F236" s="56"/>
+      <c r="G236" s="56"/>
+    </row>
+    <row r="237" ht="12.75" customHeight="1">
+      <c r="A237" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="B237" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="C237" s="59"/>
+      <c r="D237" s="59"/>
+      <c r="E237" s="59"/>
+      <c r="F237" s="59"/>
+      <c r="G237" s="60"/>
+    </row>
+    <row r="238" ht="12.75" customHeight="1">
+      <c r="A238" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="B238" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="C238" s="59"/>
+      <c r="D238" s="59"/>
+      <c r="E238" s="59"/>
+      <c r="F238" s="59"/>
+      <c r="G238" s="60"/>
+    </row>
+    <row r="239" ht="12.75" customHeight="1">
+      <c r="A239" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="B239" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="C239" s="43"/>
+      <c r="D239" s="43"/>
+      <c r="E239" s="43"/>
+      <c r="F239" s="43"/>
+      <c r="G239" s="43"/>
+    </row>
+    <row r="240" ht="12.75" customHeight="1">
+      <c r="A240" s="63"/>
+      <c r="B240" s="64"/>
+      <c r="C240" s="64"/>
+      <c r="D240" s="64"/>
+      <c r="E240" s="64"/>
+      <c r="F240" s="64"/>
+      <c r="G240" s="64"/>
+    </row>
+    <row r="241" ht="12.75" customHeight="1">
+      <c r="A241" s="65" t="s">
+        <v>19</v>
+      </c>
+      <c r="B241" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="C241" s="66" t="s">
+        <v>21</v>
+      </c>
+      <c r="D241" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="E241" s="66" t="s">
+        <v>23</v>
+      </c>
+      <c r="F241" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="G241" s="66" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="242" ht="12.75" customHeight="1">
+      <c r="A242" s="67">
+        <v>1.0</v>
+      </c>
+      <c r="B242" s="68" t="s">
+        <v>26</v>
+      </c>
+      <c r="C242" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="D242" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="E242" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="F242" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="G242" s="70" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="243" ht="12.75" customHeight="1">
+      <c r="A243" s="67">
+        <v>2.0</v>
+      </c>
+      <c r="B243" s="97" t="s">
+        <v>140</v>
+      </c>
+      <c r="C243" s="98" t="s">
+        <v>141</v>
+      </c>
+      <c r="D243" s="97" t="s">
+        <v>142</v>
+      </c>
+      <c r="E243" s="97" t="s">
+        <v>143</v>
+      </c>
+      <c r="F243" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="G243" s="104" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="244" ht="12.75" customHeight="1">
+      <c r="A244" s="67">
+        <v>3.0</v>
+      </c>
+      <c r="B244" s="104" t="s">
+        <v>133</v>
+      </c>
+      <c r="C244" s="105" t="s">
+        <v>16</v>
+      </c>
+      <c r="D244" s="104" t="s">
+        <v>28</v>
+      </c>
+      <c r="E244" s="104" t="s">
+        <v>28</v>
+      </c>
+      <c r="F244" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="G244" s="97" t="s">
+        <v>144</v>
+      </c>
+    </row>
     <row r="245" ht="12.75" customHeight="1"/>
     <row r="246" ht="12.75" customHeight="1"/>
     <row r="247" ht="12.75" customHeight="1"/>
@@ -4459,9 +5228,9 @@
     <row r="262" ht="12.75" customHeight="1"/>
     <row r="263" ht="12.75" customHeight="1"/>
     <row r="264" ht="12.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="265" ht="12.75" customHeight="1"/>
+    <row r="266" ht="12.75" customHeight="1"/>
+    <row r="267" ht="12.75" customHeight="1"/>
     <row r="268" ht="15.75" customHeight="1"/>
     <row r="269" ht="15.75" customHeight="1"/>
     <row r="270" ht="15.75" customHeight="1"/>
@@ -5197,8 +5966,9 @@
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
     <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="48">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="B7:G7"/>
@@ -5206,6 +5976,25 @@
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B22:G22"/>
     <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B66:G66"/>
+    <mergeCell ref="B67:G67"/>
+    <mergeCell ref="B81:G81"/>
+    <mergeCell ref="B82:G82"/>
+    <mergeCell ref="B97:G97"/>
+    <mergeCell ref="B98:G98"/>
+    <mergeCell ref="B113:G113"/>
+    <mergeCell ref="B114:G114"/>
+    <mergeCell ref="B127:G127"/>
+    <mergeCell ref="A167:A168"/>
+    <mergeCell ref="A183:A184"/>
+    <mergeCell ref="A202:A203"/>
+    <mergeCell ref="A217:A218"/>
+    <mergeCell ref="A232:A233"/>
     <mergeCell ref="A61:A62"/>
     <mergeCell ref="A76:A77"/>
     <mergeCell ref="A92:A93"/>
@@ -5213,14 +6002,14 @@
     <mergeCell ref="A122:A123"/>
     <mergeCell ref="A137:A138"/>
     <mergeCell ref="A152:A153"/>
-    <mergeCell ref="A167:A168"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B66:G66"/>
-    <mergeCell ref="B67:G67"/>
+    <mergeCell ref="B188:G188"/>
+    <mergeCell ref="B189:G189"/>
+    <mergeCell ref="B207:G207"/>
+    <mergeCell ref="B208:G208"/>
+    <mergeCell ref="B222:G222"/>
+    <mergeCell ref="B223:G223"/>
+    <mergeCell ref="B237:G237"/>
+    <mergeCell ref="B238:G238"/>
     <mergeCell ref="B128:G128"/>
     <mergeCell ref="B142:G142"/>
     <mergeCell ref="B143:G143"/>
@@ -5228,13 +6017,6 @@
     <mergeCell ref="B158:G158"/>
     <mergeCell ref="B172:G172"/>
     <mergeCell ref="B173:G173"/>
-    <mergeCell ref="B81:G81"/>
-    <mergeCell ref="B82:G82"/>
-    <mergeCell ref="B97:G97"/>
-    <mergeCell ref="B98:G98"/>
-    <mergeCell ref="B113:G113"/>
-    <mergeCell ref="B114:G114"/>
-    <mergeCell ref="B127:G127"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C11"/>
@@ -5253,11 +6035,12 @@
     <hyperlink r:id="rId14" ref="C163"/>
     <hyperlink r:id="rId15" ref="C177"/>
     <hyperlink r:id="rId16" ref="C178"/>
+    <hyperlink r:id="rId17" ref="C193"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId17"/>
+  <drawing r:id="rId18"/>
 </worksheet>
 </file>
 

</xml_diff>